<commit_message>
Verify Feature #176: Notification display window (start/stop dates)
- Tested date window filtering functionality
- Created notification with future start date - verified NOT visible
- Created notification with past start date - verified visible
- Created notification with expired stop date - verified NOT visible
- Tested with both admin and field_tech users
- All 7 verification steps passed
- Zero console errors
- Backend filtering logic already implemented and working correctly

Feature #176 marked as PASSING

Current progress: 174/374 features passing (46.5%)

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/.playwright-mcp/CUI-TCTO-Report-20260120.xlsx
+++ b/.playwright-mcp/CUI-TCTO-Report-20260120.xlsx
@@ -428,7 +428,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Generated: 2026-01-20 04:11:27Z</v>
+        <v>Generated: 2026-01-20 06:04:57Z</v>
       </c>
     </row>
     <row r="5">
@@ -502,7 +502,7 @@
         <v>2026-01-15Z</v>
       </c>
       <c r="H9" t="str">
-        <v>5 overdue</v>
+        <v>6 overdue</v>
       </c>
       <c r="I9" t="str">
         <v>0%</v>
@@ -540,7 +540,7 @@
         <v>2026-02-04Z</v>
       </c>
       <c r="H10" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I10" t="str">
         <v>100%</v>

</xml_diff>